<commit_message>
Fixed import investor test
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investors.xlsx
+++ b/public/sample_uploads/investors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA10C28-BAC9-4E4D-B3E6-C7287741421B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0351274-79A4-416D-AFD8-EFC5A1838C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Lake Flaviaborough</t>
   </si>
   <si>
-    <t>Tiger Global Management</t>
-  </si>
-  <si>
     <t>$100m+</t>
   </si>
   <si>
@@ -54,36 +51,24 @@
     <t>North Aracelymouth</t>
   </si>
   <si>
-    <t>Blume Ventures</t>
-  </si>
-  <si>
     <t>Cold, $100m+</t>
   </si>
   <si>
     <t>Lake Malik</t>
   </si>
   <si>
-    <t>Accel</t>
-  </si>
-  <si>
     <t>Warm</t>
   </si>
   <si>
     <t>Waiside</t>
   </si>
   <si>
-    <t>Sequoia Capital</t>
-  </si>
-  <si>
     <t>Secondary</t>
   </si>
   <si>
     <t>South Julio</t>
   </si>
   <si>
-    <t>Investor1</t>
-  </si>
-  <si>
     <t>Bangalore</t>
   </si>
   <si>
@@ -93,7 +78,22 @@
     <t>Category *</t>
   </si>
   <si>
-    <t>Kalaari Capital</t>
+    <t>Investor 1</t>
+  </si>
+  <si>
+    <t>Investor 2</t>
+  </si>
+  <si>
+    <t>Investor 3</t>
+  </si>
+  <si>
+    <t>Investor 4</t>
+  </si>
+  <si>
+    <t>Investor 5</t>
+  </si>
+  <si>
+    <t>Investor 6</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -468,13 +468,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -496,72 +496,72 @@
     </row>
     <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added pivoting in filters
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investors.xlsx
+++ b/public/sample_uploads/investors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D5B433-43A3-4AFB-9C8A-6787EE8DA392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC4EF51-64BE-46AC-864A-547024F63E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,174 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{87B218AD-CC5B-4B1E-8436-F74C80D640C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-Mandatory
+-Name you wish to record for finding investor
+- Name needs to be unique for your entity.  
+- Investing entity name can be different, which you can add in KYC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{280EF406-7F18-42B1-8927-6CEBACF1DFB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional to add Tax ID No.  
+In case available, helps combine investors added with different names
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{49EB61F4-B3BC-40EA-B9F0-8423D41D5E90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mandatory
+This is the unique identifier for each investor.  
+Note – this will not trigger any notification / access.  
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{21031F3D-3D35-46EA-9EF8-E25252F4C911}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional
+To help you find investor later  Can be whatever you want it to be! 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{2EC95963-3CD8-4C9B-A0F9-CA6C39E25CD7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mandatory
+This is to group investors in category you define.  
+Can edit Categories under the Home button / Entity details (home icon on top right)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DF26198C-A24C-4F6A-BA10-B0D4531E16B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional
+To help you find investors later.  Can be whatever you want it to be</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
@@ -90,9 +258,6 @@
     <t>Investor 6</t>
   </si>
   <si>
-    <t>PAN *</t>
-  </si>
-  <si>
     <t>BUHNXDFEA6</t>
   </si>
   <si>
@@ -105,15 +270,6 @@
     <t>4I3FNDATK0</t>
   </si>
   <si>
-    <t>TAGS</t>
-  </si>
-  <si>
-    <t>category *</t>
-  </si>
-  <si>
-    <t>Primary Email</t>
-  </si>
-  <si>
     <t>emp1@gmail.com</t>
   </si>
   <si>
@@ -130,13 +286,25 @@
   </si>
   <si>
     <t>emp6@gmail.com</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Primary Email *</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Category *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -153,6 +321,19 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -497,11 +678,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -517,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -537,10 +718,10 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -557,10 +738,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -577,10 +758,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -597,10 +778,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -618,7 +799,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -636,7 +817,7 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -665,5 +846,6 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>